<commit_message>
[MPD] V1.0 debugging Start
</commit_message>
<xml_diff>
--- a/2_Micro_Plasma_Dispenser/0_Block Diagram/MPD Block Diagram.xlsx
+++ b/2_Micro_Plasma_Dispenser/0_Block Diagram/MPD Block Diagram.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Block Diagram" sheetId="1" r:id="rId1"/>
+    <sheet name="Harness" sheetId="2" r:id="rId2"/>
+    <sheet name="HP Cable" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>KEY_PWR</t>
   </si>
@@ -163,6 +163,118 @@
   </si>
   <si>
     <t>CN200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KEY PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANS PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOOT S/W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AWG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN #</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CON P/N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ref</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>053398-0671</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,000mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOLEX-5264-6P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOLEX-5264-5P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOLEX-5264-2P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>51021-0600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내부 하네스 V1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP Cable V1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas OUT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -195,15 +307,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -327,11 +457,212 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -339,23 +670,171 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -376,10 +855,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1057405" cy="342786"/>
     <xdr:sp macro="" textlink="">
@@ -389,7 +868,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3819525" y="638175"/>
+          <a:off x="4105275" y="1143000"/>
           <a:ext cx="1057405" cy="342786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -441,14 +920,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -457,8 +936,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2552700" y="533400"/>
-          <a:ext cx="3619500" cy="7124700"/>
+          <a:off x="2552700" y="847725"/>
+          <a:ext cx="4276725" cy="7915275"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -755,6 +1234,951 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="652486" cy="593239"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9505950" y="6515100"/>
+          <a:ext cx="652486" cy="593239"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Trans</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>PCB</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7848600" y="6315074"/>
+          <a:ext cx="2924175" cy="2181226"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 5390"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="447675" y="1276350"/>
+          <a:ext cx="1362075" cy="733425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DC Adapter</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>5V, 2A</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>이상</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="오른쪽 화살표 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1971675" y="1609725"/>
+          <a:ext cx="695325" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="왼쪽 화살표 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6257925" y="1933575"/>
+          <a:ext cx="866775" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="왼쪽 화살표 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="6286500" y="3733800"/>
+          <a:ext cx="866775" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="왼쪽 화살표 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="6819900" y="7391400"/>
+          <a:ext cx="866775" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="모서리가 둥근 직사각형 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="5314950"/>
+          <a:ext cx="1362075" cy="733425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>FOOT S/W</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="왼쪽 화살표 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1819275" y="5581650"/>
+          <a:ext cx="866775" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>290514</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="왼쪽 화살표 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3286126" y="7215188"/>
+          <a:ext cx="309562" cy="223836"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="485775" y="8058150"/>
+          <a:ext cx="1362075" cy="733425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Gas Tank</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="왼쪽 화살표 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1838324" y="8410575"/>
+          <a:ext cx="866775" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57148</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1285874</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="왼쪽 화살표 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="4105273" y="8220075"/>
+          <a:ext cx="1228726" cy="104775"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>196293</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104655</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="직사각형 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AF038D3A-A707-4989-AF8C-E7A4B59D6C4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="6391275"/>
+          <a:ext cx="1453593" cy="599955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>S/V</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>0.5W</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 5VDC</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(X605SF)</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1045,16 +2469,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E5:M35"/>
+  <dimension ref="E5:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25:S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="3.875" customWidth="1"/>
     <col min="6" max="6" width="13.25" customWidth="1"/>
+    <col min="7" max="7" width="17.625" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
     <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.875" customWidth="1"/>
@@ -1063,50 +2488,50 @@
   <sheetData>
     <row r="5" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="H6" s="7" t="s">
+      <c r="F6" s="48"/>
+      <c r="H6" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="L6" s="7" t="s">
+      <c r="I6" s="48"/>
+      <c r="L6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="8"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="H7" s="12" t="s">
+      <c r="F7" s="50"/>
+      <c r="H7" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="L7" s="12" t="s">
+      <c r="I7" s="52"/>
+      <c r="L7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="13"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="L8" s="1">
         <v>1</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1165,10 +2590,10 @@
       </c>
     </row>
     <row r="12" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="54"/>
       <c r="H12" s="5">
         <v>5</v>
       </c>
@@ -1183,10 +2608,10 @@
       </c>
     </row>
     <row r="13" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="10"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="14" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E14" s="1">
@@ -1195,14 +2620,14 @@
       <c r="F14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="8"/>
-      <c r="L14" s="7" t="s">
+      <c r="I14" s="48"/>
+      <c r="L14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M14" s="8"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E15" s="3">
@@ -1211,14 +2636,14 @@
       <c r="F15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="L15" s="12" t="s">
+      <c r="I15" s="52"/>
+      <c r="L15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="M15" s="13"/>
+      <c r="M15" s="11"/>
     </row>
     <row r="16" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E16" s="3">
@@ -1230,13 +2655,13 @@
       <c r="H16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L16" s="1">
         <v>1</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1275,10 +2700,10 @@
       </c>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="58"/>
       <c r="H19" s="3">
         <v>4</v>
       </c>
@@ -1293,10 +2718,10 @@
       </c>
     </row>
     <row r="20" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="10"/>
+      <c r="F20" s="60"/>
       <c r="H20" s="3">
         <v>5</v>
       </c>
@@ -1311,10 +2736,10 @@
       </c>
     </row>
     <row r="21" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="1">
+      <c r="E21" s="61">
         <v>1</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="62" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="5">
@@ -1330,68 +2755,41 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="3">
+    <row r="22" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E22" s="63">
         <v>2</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="64" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="5">
+      <c r="E23" s="65">
         <v>3</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="13"/>
-    </row>
+    </row>
+    <row r="24" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="H25" s="1">
-        <v>1</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>24</v>
-      </c>
+      <c r="F25" s="48"/>
     </row>
     <row r="26" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="H26" s="3">
-        <v>2</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F26" s="50"/>
     </row>
     <row r="27" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="H27" s="3">
-        <v>3</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="28" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1401,60 +2799,183 @@
       <c r="F28" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H28" s="3">
+    </row>
+    <row r="29" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="48"/>
+    </row>
+    <row r="31" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E31" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="50"/>
+      <c r="H31" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="48"/>
+      <c r="L31" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="M31" s="9"/>
+    </row>
+    <row r="32" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="52"/>
+      <c r="L32" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="M32" s="11"/>
+    </row>
+    <row r="33" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E33" s="5">
+        <v>2</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="1">
+        <v>6</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="H34" s="3">
+        <v>2</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="3">
+        <v>5</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="H35" s="3">
+        <v>3</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35" s="3">
         <v>4</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="M35" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E36" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="56"/>
+      <c r="H36" s="3">
+        <v>4</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="H29" s="3">
+      <c r="L36" s="3">
+        <v>3</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="3">
         <v>5</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I37" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H30" s="5">
+      <c r="L37" s="3">
+        <v>2</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E38" s="5">
+        <v>2</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="5">
         <v>6</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I38" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="H32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="8"/>
-    </row>
-    <row r="33" spans="8:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H33" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" s="10"/>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H34" s="1">
+      <c r="L38" s="5">
         <v>1</v>
       </c>
-      <c r="I34" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="8:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H35" s="5">
-        <v>2</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="M38" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E39" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="68"/>
+      <c r="H39" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I39" s="13"/>
+      <c r="L39" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="M39" s="13"/>
+    </row>
+    <row r="40" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E40" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="27">
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="E26:F26"/>
@@ -1464,17 +2985,13 @@
     <mergeCell ref="L15:M15"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1485,12 +3002,476 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9" style="18"/>
+    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.75" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" customWidth="1"/>
+    <col min="8" max="8" width="14.75" customWidth="1"/>
+    <col min="9" max="9" width="6.75" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" customWidth="1"/>
+    <col min="13" max="13" width="9" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="27">
+        <v>1</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="26"/>
+      <c r="I5" s="27">
+        <v>1</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="30"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20">
+        <v>2</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="20">
+        <v>2</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="31"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="30"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20">
+        <v>3</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20">
+        <v>3</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="31"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="30"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20">
+        <v>4</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20">
+        <v>4</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="31"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="30"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20">
+        <v>5</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20">
+        <v>5</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="31"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="30"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20">
+        <v>6</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="20">
+        <v>6</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="31"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="20">
+        <v>1</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="20">
+        <v>1</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="30"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20">
+        <v>2</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="20">
+        <v>2</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="31"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="30"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20">
+        <v>3</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="20">
+        <v>3</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="31"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="30"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20">
+        <v>4</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="20">
+        <v>4</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="31"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="30"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20">
+        <v>5</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="20">
+        <v>5</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="31"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="20">
+        <v>1</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="20">
+        <v>1</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="30"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20">
+        <v>2</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20">
+        <v>2</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="32"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="20">
+        <v>1</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="19"/>
+      <c r="I18" s="20">
+        <v>1</v>
+      </c>
+      <c r="J18" s="21"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35">
+        <v>2</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="42"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="35">
+        <v>2</v>
+      </c>
+      <c r="J19" s="35"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="G5:G10"/>
+    <mergeCell ref="H5:H10"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="K5:K10"/>
+    <mergeCell ref="K11:K15"/>
+    <mergeCell ref="L11:L15"/>
+    <mergeCell ref="L5:L10"/>
+    <mergeCell ref="M11:M15"/>
+    <mergeCell ref="M5:M10"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C5:C10"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="D5:D10"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1498,12 +3479,241 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9" style="18"/>
+    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.75" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" customWidth="1"/>
+    <col min="8" max="8" width="14.75" customWidth="1"/>
+    <col min="9" max="9" width="6.75" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" customWidth="1"/>
+    <col min="13" max="13" width="9" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20">
+        <v>6</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="30"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20">
+        <v>2</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="41"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="20">
+        <v>5</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="31"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="30"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20">
+        <v>3</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="41"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20">
+        <v>4</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="31"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="30"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20">
+        <v>4</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="41"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20">
+        <v>3</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="31"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="30"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20">
+        <v>5</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="41"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20">
+        <v>2</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="31"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="30"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20">
+        <v>6</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="20">
+        <v>1</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="31"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="69"/>
+      <c r="I11" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="L5:L10"/>
+    <mergeCell ref="M5:M10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="C5:C10"/>
+    <mergeCell ref="D5:D10"/>
+    <mergeCell ref="G5:G10"/>
+    <mergeCell ref="H5:H10"/>
+    <mergeCell ref="K5:K10"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>